<commit_message>
started emulator and added instructions
</commit_message>
<xml_diff>
--- a/Architecture.xlsx
+++ b/Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\Stuff\Nonsense\CPU_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42F70D7-D468-45FC-9592-E12572137F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF32E1-A768-4E1F-96FB-A9D1F90FAD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Insutrctions" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="111">
   <si>
     <t>NOP</t>
   </si>
@@ -198,9 +198,6 @@
     <t>STC</t>
   </si>
   <si>
-    <t>(write data from register C into RAM location) parameter: 16-bit RAM address</t>
-  </si>
-  <si>
     <t>Heading</t>
   </si>
   <si>
@@ -237,15 +234,9 @@
     <t>LDD</t>
   </si>
   <si>
-    <t>(read data from RAM location into register D) parameter: 16-bit RAM address</t>
-  </si>
-  <si>
     <t>STD</t>
   </si>
   <si>
-    <t>(write data from register D into RAM location) parameter: 16-bit RAM address</t>
-  </si>
-  <si>
     <t>Flags</t>
   </si>
   <si>
@@ -334,6 +325,51 @@
   </si>
   <si>
     <t>4 bit</t>
+  </si>
+  <si>
+    <t>Memory MAP</t>
+  </si>
+  <si>
+    <t>BIOS</t>
+  </si>
+  <si>
+    <t>While in bios mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 bit: </t>
+  </si>
+  <si>
+    <t>0-1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32bit </t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>STE</t>
+  </si>
+  <si>
+    <t>LDE</t>
+  </si>
+  <si>
+    <t>(write data from Accumlator into RAM location) parameter: 16-bit RAM address</t>
+  </si>
+  <si>
+    <t>(write data from Segment register into RAM location) parameter: 16-bit RAM address</t>
+  </si>
+  <si>
+    <t>(read data from RAM location into Segment register) parameter: 16-bit RAM address</t>
+  </si>
+  <si>
+    <t>(read data from RAM location into Flag register) parameter: 16-bit RAM address</t>
+  </si>
+  <si>
+    <t>(write data from Flag register into RAM location) parameter: 16-bit RAM address</t>
   </si>
 </sst>
 </file>
@@ -660,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,13 +711,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
@@ -713,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C35" si="0">DEC2HEX(B3, 2)</f>
+        <f t="shared" ref="C3:C37" si="0">DEC2HEX(B3, 2)</f>
         <v>01</v>
       </c>
       <c r="D3" t="s">
@@ -741,7 +777,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <f t="shared" ref="B5:B34" si="1">B4+1</f>
+        <f t="shared" ref="B5:B36" si="1">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" t="str">
@@ -749,10 +785,10 @@
         <v>03</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -765,15 +801,15 @@
         <v>04</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f>B6+1</f>
         <v>5</v>
       </c>
       <c r="C7" t="str">
@@ -781,10 +817,10 @@
         <v>05</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -797,10 +833,10 @@
         <v>06</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -813,10 +849,10 @@
         <v>07</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -829,10 +865,10 @@
         <v>08</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -845,29 +881,26 @@
         <v>09</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
       <c r="B12">
         <f>B11+1</f>
         <v>10</v>
       </c>
       <c r="C12" t="str">
-        <f>DEC2HEX(B12, 2)</f>
+        <f t="shared" si="0"/>
         <v>0A</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -880,26 +913,29 @@
         <v>0B</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f>B13+1</f>
         <v>12</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(B14, 2)</f>
         <v>0C</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,10 +948,10 @@
         <v>0D</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -928,10 +964,10 @@
         <v>0E</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -944,10 +980,10 @@
         <v>0F</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -960,10 +996,10 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -976,29 +1012,26 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <f>B19+1</f>
-        <v>18</v>
-      </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1011,15 +1044,18 @@
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f>B21+1</f>
         <v>20</v>
       </c>
       <c r="C22" t="str">
@@ -1027,10 +1063,10 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1043,10 +1079,10 @@
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1059,10 +1095,10 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1075,10 +1111,10 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1091,10 +1127,10 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1107,18 +1143,15 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
       <c r="B28">
-        <f>B27+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C28" t="str">
@@ -1126,10 +1159,10 @@
         <v>1A</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1142,15 +1175,18 @@
         <v>1B</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f>B29+1</f>
         <v>28</v>
       </c>
       <c r="C30" t="str">
@@ -1158,10 +1194,10 @@
         <v>1C</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1174,10 +1210,10 @@
         <v>1D</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1190,10 +1226,10 @@
         <v>1E</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1206,10 +1242,10 @@
         <v>1F</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1222,18 +1258,15 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>96</v>
-      </c>
       <c r="B35">
-        <f>B34+1</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C35" t="str">
@@ -1241,26 +1274,61 @@
         <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36">
-        <f>B35+1</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36" si="2">DEC2HEX(B36, 2)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37">
+        <f>B36+1</f>
+        <v>35</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <f>B37+1</f>
+        <v>36</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" ref="C38" si="2">DEC2HEX(B38, 2)</f>
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1271,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7175E51-51B0-45A8-B4A4-78E4198A6F1F}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,94 +1353,128 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>97</v>
+      <c r="B14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>